<commit_message>
test_get.py done - Arek
</commit_message>
<xml_diff>
--- a/docs/cases_api.xlsx
+++ b/docs/cases_api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arkadiusz/1.MyAllFiles/1.Studies/7th_Semester/JPWO/jpwo-qa-automation-py/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28C284C2-A46A-D24A-A8A3-CD9ECB75C9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30054247-8EA6-384B-A062-E1A9D339D443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16240" yWindow="3760" windowWidth="28040" windowHeight="17180" xr2:uid="{EF56D35B-1259-5E47-A7BC-09AB8A8339D5}"/>
+    <workbookView xWindow="46860" yWindow="620" windowWidth="13620" windowHeight="24720" xr2:uid="{EF56D35B-1259-5E47-A7BC-09AB8A8339D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>LP</t>
+  </si>
+  <si>
+    <t>Nazwa testu</t>
+  </si>
+  <si>
+    <t>Kategoria</t>
+  </si>
+  <si>
+    <t>Krótki opis</t>
+  </si>
+  <si>
+    <t>test_get_product_happy</t>
+  </si>
+  <si>
+    <t>test_get_product_negative_valid_input_not_found</t>
+  </si>
+  <si>
+    <t>happy tests</t>
+  </si>
+  <si>
+    <t>negative testing with valid input</t>
+  </si>
+  <si>
+    <t>sprawdza czy zwraca poprawnie istniejący produkt, kod 200</t>
+  </si>
+  <si>
+    <t>sprawdza czy api poprawnie zwraca kod błędu 404 dla nie istniejącego produktu</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -45,16 +80,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +110,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +472,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D56F03-1724-3141-A046-4D40772A6DE2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test_put.py Done - Arek
</commit_message>
<xml_diff>
--- a/docs/cases_api.xlsx
+++ b/docs/cases_api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arkadiusz/1.MyAllFiles/1.Studies/7th_Semester/JPWO/jpwo-qa-automation-py/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1919041-1B89-7446-BAF7-049AFE77A733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819A8E4D-03DD-384F-B20A-475A47590D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16740" yWindow="26020" windowWidth="27280" windowHeight="16380" xr2:uid="{EF56D35B-1259-5E47-A7BC-09AB8A8339D5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>LP</t>
   </si>
@@ -90,6 +90,27 @@
   </si>
   <si>
     <t>sprawdza czy api poprawnie zwraca kod błędu przy próbie dodania produktu z pustym body</t>
+  </si>
+  <si>
+    <t>test_put_product_happy</t>
+  </si>
+  <si>
+    <t>test_put_product_negative_valid_input_not_found</t>
+  </si>
+  <si>
+    <t>test_put_product_negative_invalid_input_schema</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>sprawdza czy api poprawnie zwraca kod błędu przy próbie błędnej aktualizacji danych</t>
+  </si>
+  <si>
+    <t>sprawdza czy api zwraca poprawny kod błędu przy próbie aktualizacji nieistniejącego produktu</t>
+  </si>
+  <si>
+    <t>sprawdza czy api poprawnie zwraca kod oraz aktualizuje zasób</t>
   </si>
 </sst>
 </file>
@@ -500,7 +521,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,32 +618,56 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">

</xml_diff>

<commit_message>
test_delete.py done - Arek #2
</commit_message>
<xml_diff>
--- a/docs/cases_api.xlsx
+++ b/docs/cases_api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arkadiusz/1.MyAllFiles/1.Studies/7th_Semester/JPWO/jpwo-qa-automation-py/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819A8E4D-03DD-384F-B20A-475A47590D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171EAFD5-90AF-0348-A47F-4A6A38FE459F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16740" yWindow="26020" windowWidth="27280" windowHeight="16380" xr2:uid="{EF56D35B-1259-5E47-A7BC-09AB8A8339D5}"/>
   </bookViews>
@@ -36,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
-  <si>
-    <t>LP</t>
-  </si>
-  <si>
-    <t>Nazwa testu</t>
-  </si>
-  <si>
-    <t>Kategoria</t>
-  </si>
-  <si>
-    <t>Krótki opis</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>test_get_product_happy</t>
   </si>
@@ -62,18 +50,9 @@
     <t>negative testing with valid input</t>
   </si>
   <si>
-    <t>sprawdza czy zwraca poprawnie istniejący produkt, kod 200</t>
-  </si>
-  <si>
-    <t>sprawdza czy api poprawnie zwraca kod błędu 404 dla nie istniejącego produktu</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
-    <t>Metoda</t>
-  </si>
-  <si>
     <t>test_post_product_happy</t>
   </si>
   <si>
@@ -86,12 +65,6 @@
     <t>negative testing with invalid input</t>
   </si>
   <si>
-    <t>sprawdza czy api zwraca poprawny kod przy dodaniu nowego produktu</t>
-  </si>
-  <si>
-    <t>sprawdza czy api poprawnie zwraca kod błędu przy próbie dodania produktu z pustym body</t>
-  </si>
-  <si>
     <t>test_put_product_happy</t>
   </si>
   <si>
@@ -104,13 +77,73 @@
     <t>PUT</t>
   </si>
   <si>
-    <t>sprawdza czy api poprawnie zwraca kod błędu przy próbie błędnej aktualizacji danych</t>
-  </si>
-  <si>
-    <t>sprawdza czy api zwraca poprawny kod błędu przy próbie aktualizacji nieistniejącego produktu</t>
-  </si>
-  <si>
-    <t>sprawdza czy api poprawnie zwraca kod oraz aktualizuje zasób</t>
+    <t>test_delete_product_happy</t>
+  </si>
+  <si>
+    <t>test_delete_product_negative_valid_input_not_found</t>
+  </si>
+  <si>
+    <t>test_delete_product_negative_product_used_elsewhere</t>
+  </si>
+  <si>
+    <t>test_delete_product_negative_unauthorized</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Pobiera listę produktów, wybiera pierwszy i sprawdza GET po jego id; oczekuje 200 i kluczowych pól w JSON.</t>
+  </si>
+  <si>
+    <t>Próba pobrania nieistniejącego produktu; oczekuje 404.</t>
+  </si>
+  <si>
+    <t>Dodaje nowy produkt poprawnym payloadem; zgodnie ze spec oczekuje 200 (test oznacza xfail, gdy implementacja zwraca 201).</t>
+  </si>
+  <si>
+    <t>Próba dodania produktu z niepoprawnym body (np. puste „name”); oczekuje 422.</t>
+  </si>
+  <si>
+    <t>Aktualizuje istniejący produkt (zmiana „name”); oczekuje 200 i weryfikuje aktualizację przez GET.</t>
+  </si>
+  <si>
+    <t>Aktualizacja nieistniejącego produktu przy poprawnym payloadzie; zgodnie ze spec oczekuje 404 (gdy implementacja zwraca 200 z success=false, test oznaczany xfail).</t>
+  </si>
+  <si>
+    <t>Aktualizacja istniejącego produktu niepoprawnym payloadem; oczekuje 422.</t>
+  </si>
+  <si>
+    <t>Usuwa świeżo utworzony produkt; zgodnie ze spec oczekuje 204.</t>
+  </si>
+  <si>
+    <t>Drugie usunięcie tego samego id (po wcześniejszym 204); zgodnie ze spec oczekuje 404 (xfail, gdy środowisko zwraca 200 z success=false lub 422).</t>
+  </si>
+  <si>
+    <t>Usunięcie z niepoprawnym id w ścieżce (np. „abc”); oczekuje 422.</t>
+  </si>
+  <si>
+    <t>Próba usunięcia istniejącego produktu powiązanego w systemie; oczekuje 409.</t>
+  </si>
+  <si>
+    <t>Usunięcie bez autoryzacji; oczekuje 401.</t>
+  </si>
+  <si>
+    <t>Test name</t>
+  </si>
+  <si>
+    <t>Test category</t>
+  </si>
+  <si>
+    <t>Short description (in polish)</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>test_delete_product_negative_invalid_input_non_uuid</t>
   </si>
 </sst>
 </file>
@@ -133,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +176,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,8 +213,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -184,6 +224,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,237 +563,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D56F03-1724-3141-A046-4D40772A6DE2}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="3" max="3" width="47.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="E10" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="E11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B20" s="1"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test_delete.py done - Arek #3
</commit_message>
<xml_diff>
--- a/docs/cases_api.xlsx
+++ b/docs/cases_api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arkadiusz/1.MyAllFiles/1.Studies/7th_Semester/JPWO/jpwo-qa-automation-py/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171EAFD5-90AF-0348-A47F-4A6A38FE459F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02F5C6C-E852-C146-B735-E40517F43F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16740" yWindow="26020" windowWidth="27280" windowHeight="16380" xr2:uid="{EF56D35B-1259-5E47-A7BC-09AB8A8339D5}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Próba pobrania nieistniejącego produktu; oczekuje 404.</t>
   </si>
   <si>
-    <t>Dodaje nowy produkt poprawnym payloadem; zgodnie ze spec oczekuje 200 (test oznacza xfail, gdy implementacja zwraca 201).</t>
-  </si>
-  <si>
     <t>Próba dodania produktu z niepoprawnym body (np. puste „name”); oczekuje 422.</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>test_delete_product_negative_invalid_input_non_uuid</t>
+  </si>
+  <si>
+    <t>Dodaje nowy produkt poprawnym payloadem; zgodnie ze spec oczekuje 200.</t>
   </si>
 </sst>
 </file>
@@ -223,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -566,7 +566,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,19 +580,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -643,7 +643,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -677,7 +677,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -694,7 +694,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -711,7 +711,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -728,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -756,13 +756,13 @@
         <v>17</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -779,7 +779,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>